<commit_message>
full load logic - weights and scores
</commit_message>
<xml_diff>
--- a/scores-from-excel/jane-romco-scores.xlsx
+++ b/scores-from-excel/jane-romco-scores.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+  <si>
+    <t>Scale</t>
+  </si>
   <si>
     <t>Scorer</t>
   </si>
@@ -20,9 +23,6 @@
     <t>Jane Doe</t>
   </si>
   <si>
-    <t>Scale</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -53,49 +53,55 @@
     <t>Bad</t>
   </si>
   <si>
+    <t>Hold time less than 5 minutes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Must be able to hold 20 oz </t>
   </si>
   <si>
-    <t>Hold time less than 5 minutes</t>
-  </si>
-  <si>
     <t>Meh</t>
   </si>
   <si>
+    <t>Resolution on first call</t>
+  </si>
+  <si>
+    <t>Very Good</t>
+  </si>
+  <si>
     <t>Flexible</t>
   </si>
   <si>
-    <t>Resolution on first call</t>
-  </si>
-  <si>
-    <t>Very Good</t>
-  </si>
-  <si>
     <t>Gizmos to the wingnut</t>
   </si>
   <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>Packaging</t>
+  </si>
+  <si>
     <t>Polite</t>
   </si>
   <si>
-    <t>Excellent</t>
-  </si>
-  <si>
-    <t>Packaging</t>
+    <t>Pleasant apppearance</t>
   </si>
   <si>
     <t>Corporate Viability</t>
   </si>
   <si>
-    <t>Pleasant apppearance</t>
-  </si>
-  <si>
     <t>Easy to open</t>
   </si>
   <si>
+    <t>Cut my finger</t>
+  </si>
+  <si>
     <t>D&amp;B Rating</t>
   </si>
   <si>
     <t>Recyclable</t>
+  </si>
+  <si>
+    <t>Made from toxic sludge</t>
   </si>
   <si>
     <t>Years in business</t>
@@ -170,11 +176,11 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -211,25 +217,26 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="28.43"/>
+    <col customWidth="1" min="3" max="3" width="20.29"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="F2" s="3"/>
     </row>
@@ -242,7 +249,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="4">
@@ -271,7 +278,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4">
         <v>5.0</v>
@@ -286,7 +293,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4">
         <v>4.0</v>
@@ -296,7 +303,7 @@
         <v>4.0</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -311,12 +318,12 @@
         <v>5.0</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11">
@@ -332,7 +339,7 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="4">
         <v>3.0</v>
@@ -346,16 +353,20 @@
       <c r="B13" s="4">
         <v>2.0</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="4">
         <v>0.0</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -384,8 +395,8 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="E2" s="2" t="s">
-        <v>2</v>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="F2" s="3"/>
     </row>
@@ -398,7 +409,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="4">
@@ -427,7 +438,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="4">
         <v>2.0</v>
@@ -442,7 +453,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4">
         <v>4.0</v>
@@ -452,12 +463,12 @@
         <v>4.0</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="4">
         <v>2.0</v>
@@ -467,12 +478,12 @@
         <v>5.0</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
+      <c r="A10" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11">
@@ -488,7 +499,7 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4">
         <v>3.0</v>
@@ -497,7 +508,7 @@
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B13" s="4">
         <v>3.0</v>

</xml_diff>

<commit_message>
messing with aggregates and pandas
</commit_message>
<xml_diff>
--- a/scores-from-excel/jane-romco-scores.xlsx
+++ b/scores-from-excel/jane-romco-scores.xlsx
@@ -12,14 +12,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+  <si>
+    <t>Scorer</t>
+  </si>
   <si>
     <t>Scale</t>
   </si>
   <si>
-    <t>Scorer</t>
-  </si>
-  <si>
     <t>Jane Doe</t>
   </si>
   <si>
@@ -62,27 +62,27 @@
     <t>Meh</t>
   </si>
   <si>
+    <t>Flexible</t>
+  </si>
+  <si>
     <t>Resolution on first call</t>
   </si>
   <si>
     <t>Very Good</t>
   </si>
   <si>
-    <t>Flexible</t>
-  </si>
-  <si>
     <t>Gizmos to the wingnut</t>
   </si>
   <si>
     <t>Excellent</t>
   </si>
   <si>
+    <t>Polite</t>
+  </si>
+  <si>
     <t>Packaging</t>
   </si>
   <si>
-    <t>Polite</t>
-  </si>
-  <si>
     <t>Pleasant apppearance</t>
   </si>
   <si>
@@ -92,19 +92,22 @@
     <t>Easy to open</t>
   </si>
   <si>
+    <t>D&amp;B Rating</t>
+  </si>
+  <si>
     <t>Cut my finger</t>
   </si>
   <si>
-    <t>D&amp;B Rating</t>
+    <t>No time to check</t>
   </si>
   <si>
     <t>Recyclable</t>
   </si>
   <si>
+    <t>Years in business</t>
+  </si>
+  <si>
     <t>Made from toxic sludge</t>
-  </si>
-  <si>
-    <t>Years in business</t>
   </si>
 </sst>
 </file>
@@ -176,11 +179,11 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -221,22 +224,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="F2" s="3"/>
     </row>
@@ -249,7 +252,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="4">
@@ -293,7 +296,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4">
         <v>4.0</v>
@@ -303,7 +306,7 @@
         <v>4.0</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
@@ -322,8 +325,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>21</v>
+      <c r="A10" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11">
@@ -354,18 +357,18 @@
         <v>2.0</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" s="4">
         <v>0.0</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -395,8 +398,8 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="E2" s="1" t="s">
-        <v>0</v>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="F2" s="3"/>
     </row>
@@ -409,7 +412,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="4">
@@ -453,7 +456,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4">
         <v>4.0</v>
@@ -463,12 +466,12 @@
         <v>4.0</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="4">
         <v>2.0</v>
@@ -482,7 +485,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -499,12 +502,12 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="C12" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">

</xml_diff>